<commit_message>
Add b parameter plots using R
</commit_message>
<xml_diff>
--- a/Data/plots/pcm/par_LaTeX.xlsx
+++ b/Data/plots/pcm/par_LaTeX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Data\plots\pcm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DC59DE-67B9-4C0B-9F9A-C02275649E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB6C60E-F2E2-4BB6-A47B-9B51D30FCF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{64DB1CC6-AF11-4A36-8697-4EDD54E50872}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
   <si>
     <t>Subject Code</t>
   </si>
@@ -307,6 +307,39 @@
   </si>
   <si>
     <t>Oral Norwegian</t>
+  </si>
+  <si>
+    <t>ENG_W</t>
+  </si>
+  <si>
+    <t>MAT_W</t>
+  </si>
+  <si>
+    <t>NOR_W</t>
+  </si>
+  <si>
+    <t>ENG_O</t>
+  </si>
+  <si>
+    <t>NOR_O</t>
+  </si>
+  <si>
+    <t>MAT</t>
+  </si>
+  <si>
+    <t>[Exam] Mathematics</t>
+  </si>
+  <si>
+    <t>[Exam] Written English</t>
+  </si>
+  <si>
+    <t>[Exam] Written Norwegian</t>
+  </si>
+  <si>
+    <t>[Exam] Oral English</t>
+  </si>
+  <si>
+    <t>[Exam] Oral Norwegian</t>
   </si>
 </sst>
 </file>
@@ -336,7 +369,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -364,20 +397,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,41 +424,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,6 +551,86 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>graph!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>b1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>b2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>b4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>b5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.7969999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.752</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.13500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-752F-4582-B3CE-85BEEF61D93E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>Written Norwegian</c:v>
                 </c:pt>
               </c:strCache>
@@ -559,84 +648,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.227411731998888E-2"/>
-                  <c:y val="-3.1347967540948589E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000017-752F-4582-B3CE-85BEEF61D93E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>graph!$C$1:$G$1</c:f>
@@ -662,24 +673,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$2:$G$2</c:f>
+              <c:f>graph!$C$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-5.9530000000000003</c:v>
+                  <c:v>-5.4669999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.0619999999999998</c:v>
+                  <c:v>-2.7759999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.80500000000000005</c:v>
+                  <c:v>-0.68100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2050000000000001</c:v>
+                  <c:v>1.266</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.605</c:v>
+                  <c:v>3.613</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -687,16 +698,258 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-752F-4582-B3CE-85BEEF61D93E}"/>
+              <c16:uniqueId val="{00000001-752F-4582-B3CE-85BEEF61D93E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>graph!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Written English</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>graph!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>b1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>b2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>b4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>b5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.8230000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.7040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.89200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0209999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-752F-4582-B3CE-85BEEF61D93E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Natural Sciences</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>graph!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>b1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>b2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>b4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>b5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-5.4859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.9209999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4609999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-752F-4582-B3CE-85BEEF61D93E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Religion and Ethics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>graph!$C$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>b1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>b2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>b4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>b5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-5.5869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.177</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3570000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-752F-4582-B3CE-85BEEF61D93E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -742,506 +995,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$3:$G$3</c:f>
+              <c:f>graph!$C$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-6.3129999999999997</c:v>
+                  <c:v>-6.1109999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.7240000000000002</c:v>
+                  <c:v>-3.5150000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.633</c:v>
+                  <c:v>-1.494</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24199999999999999</c:v>
+                  <c:v>0.32100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6219999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-752F-4582-B3CE-85BEEF61D93E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>graph!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Written English</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>graph!$C$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>b1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>b2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>b3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>b4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>b5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>graph!$C$4:$G$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-5.1890000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.9670000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1.0169999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.95699999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.1379999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-752F-4582-B3CE-85BEEF61D93E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>graph!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Oral English</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>graph!$C$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>b1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>b2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>b3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>b4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>b5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>graph!$C$5:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-5.6550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.9180000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1.788</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6179999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-752F-4582-B3CE-85BEEF61D93E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>graph!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mathematics</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-4.3887154557328105E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-752F-4582-B3CE-85BEEF61D93E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.0774248646202477E-17"/>
-                  <c:y val="-3.1347967540948665E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-752F-4582-B3CE-85BEEF61D93E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-3.1347967540948589E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-752F-4582-B3CE-85BEEF61D93E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-3.7617561049138312E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000010-752F-4582-B3CE-85BEEF61D93E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.8904642757853769E-2"/>
-                  <c:y val="-5.8516206076437351E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000011-752F-4582-B3CE-85BEEF61D93E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>graph!$C$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>b1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>b2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>b3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>b4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>b5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>graph!$C$6:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-4.9340000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.8560000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.21299999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.111</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.028</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-752F-4582-B3CE-85BEEF61D93E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>graph!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Natural Sciences</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>graph!$C$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>b1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>b2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>b3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>b4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>b5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>graph!$C$7:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-5.7240000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.085</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1.226</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.34499999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4329999999999998</c:v>
+                  <c:v>2.6520000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1258,7 +1029,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>graph!$B$8</c:f>
+              <c:f>graph!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1306,24 +1077,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$8:$G$8</c:f>
+              <c:f>graph!$C$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-6.0650000000000004</c:v>
+                  <c:v>-5.8449999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.5190000000000001</c:v>
+                  <c:v>-3.3439999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.6379999999999999</c:v>
+                  <c:v>-1.516</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0999999999999994E-2</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3330000000000002</c:v>
+                  <c:v>2.3639999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,11 +1111,11 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>graph!$B$9</c:f>
+              <c:f>graph!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Religion and Ethics</c:v>
+                  <c:v>Oral English</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1352,9 +1123,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1388,24 +1157,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$9:$G$9</c:f>
+              <c:f>graph!$C$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-5.8220000000000001</c:v>
+                  <c:v>-5.3209999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.3740000000000001</c:v>
+                  <c:v>-3.3210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.583</c:v>
+                  <c:v>-1.6319999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.152</c:v>
+                  <c:v>0.38800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3250000000000002</c:v>
+                  <c:v>2.6419999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,19 +1244,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-6.3049999999999997</c:v>
+                  <c:v>-6.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.2880000000000003</c:v>
+                  <c:v>-4.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.4710000000000001</c:v>
+                  <c:v>-2.319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.19800000000000001</c:v>
+                  <c:v>-0.11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5569999999999999</c:v>
+                  <c:v>2.589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1557,19 +1326,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-6.4470000000000001</c:v>
+                  <c:v>-6.2380000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.5990000000000002</c:v>
+                  <c:v>-4.4169999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.5219999999999998</c:v>
+                  <c:v>-2.3820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.14299999999999999</c:v>
+                  <c:v>-5.7000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6869999999999998</c:v>
+                  <c:v>2.7160000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,7 +1355,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>graph!$B$12</c:f>
+              <c:f>graph!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1614,14 +1383,14 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="1.8808780524569156E-2"/>
+                  <c:x val="5.8447480178696269E-2"/>
+                  <c:y val="2.4439918533604787E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
+              <c:showSerName val="1"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
@@ -1633,18 +1402,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.2240756185710722E-3"/>
-                  <c:y val="2.5078374032758796E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1654,18 +1412,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="3.1347967540948513E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1675,18 +1422,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="4.3887154557327952E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1696,18 +1432,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.6680567139282735E-2"/>
-                  <c:y val="5.4336477070977558E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1747,7 +1472,7 @@
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
+            <c:showSerName val="1"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
@@ -1796,24 +1521,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$12:$G$12</c:f>
+              <c:f>graph!$C$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-7.7679999999999998</c:v>
+                  <c:v>-7.58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.4550000000000001</c:v>
+                  <c:v>-5.2169999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.7909999999999999</c:v>
+                  <c:v>-2.6320000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.33600000000000002</c:v>
+                  <c:v>-0.24199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4849999999999999</c:v>
+                  <c:v>2.5169999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1830,7 +1555,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>graph!$B$13</c:f>
+              <c:f>graph!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1878,24 +1603,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$13:$G$13</c:f>
+              <c:f>graph!$C$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-6.2210000000000001</c:v>
+                  <c:v>-6.0220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.6070000000000002</c:v>
+                  <c:v>-4.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.0350000000000001</c:v>
+                  <c:v>-2.8820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.73</c:v>
+                  <c:v>-0.63400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2650000000000001</c:v>
+                  <c:v>2.3039999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1904,6 +1629,660 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-752F-4582-B3CE-85BEEF61D93E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[Exam] Mathematics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$16:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.8630000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.7589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.464</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9118-48D0-8AF2-6931004593EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[Exam] Written English</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.38356101340222E-2"/>
+                  <c:y val="-0.154786150712831"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.5819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.4129999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.32600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.526</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.355</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-9118-48D0-8AF2-6931004593EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[Exam] Written Norwegian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.19360727809193137"/>
+                  <c:y val="-1.9008825526137134E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$22:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.7249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55800000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4940000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3440000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-9118-48D0-8AF2-6931004593EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[Exam] Oral English</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$25:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-5.7030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.8119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.849</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2110000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-9118-48D0-8AF2-6931004593EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graph!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[Exam] Oral Norwegian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.4977155290381574E-2"/>
+                  <c:y val="0.13306177868295996"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-9118-48D0-8AF2-6931004593EA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>graph!$C$28:$G$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-6.0060000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.4810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.228</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-9118-48D0-8AF2-6931004593EA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1929,7 +2308,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2210,32 +2589,32 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>graph!$B$2:$B$13</c:f>
+              <c:f>graph!$B$2:$B$28</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Written Norwegian</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>Natural Sciences</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Religion and Ethics</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social Sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Oral Norwegian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Written English</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oral English</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mathematics</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Natural Sciences</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Social Sciences</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Religion and Ethics</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Music</c:v>
@@ -2244,55 +2623,115 @@
                   <c:v>Arts and Handcraft</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Physical Education</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Food and Health</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Physical Education</c:v>
+                <c:pt idx="13">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>[Exam] Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[Exam] Written English</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[Exam] Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>[Exam] Oral English</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Oral Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>[Exam] Oral Norwegian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$C$2:$C$13</c:f>
+              <c:f>graph!$C$2:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-5.9530000000000003</c:v>
+                  <c:v>-4.7969999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-6.3129999999999997</c:v>
+                  <c:v>-4.8230000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.1890000000000001</c:v>
+                  <c:v>-5.4669999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.6550000000000002</c:v>
+                  <c:v>-5.4859999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.9340000000000002</c:v>
+                  <c:v>-5.5869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.7240000000000002</c:v>
+                  <c:v>-5.8449999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6.0650000000000004</c:v>
+                  <c:v>-5.3209999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.8220000000000001</c:v>
+                  <c:v>-6.1109999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6.3049999999999997</c:v>
+                  <c:v>-6.11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-6.4470000000000001</c:v>
+                  <c:v>-6.2380000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7.7679999999999998</c:v>
+                  <c:v>-6.0220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-6.2210000000000001</c:v>
+                  <c:v>-7.58</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.7969999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.8630000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.8230000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-4.5819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-5.4669999999999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4.7249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5.3209999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-5.7030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-6.1109999999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-6.0060000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,32 +2771,32 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>graph!$B$2:$B$13</c:f>
+              <c:f>graph!$B$2:$B$28</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Written Norwegian</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>Natural Sciences</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Religion and Ethics</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social Sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Oral Norwegian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Written English</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oral English</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mathematics</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Natural Sciences</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Social Sciences</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Religion and Ethics</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Music</c:v>
@@ -2366,55 +2805,115 @@
                   <c:v>Arts and Handcraft</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Physical Education</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Food and Health</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Physical Education</c:v>
+                <c:pt idx="13">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>[Exam] Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[Exam] Written English</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[Exam] Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>[Exam] Oral English</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Oral Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>[Exam] Oral Norwegian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$D$2:$D$13</c:f>
+              <c:f>graph!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-3.0619999999999998</c:v>
+                  <c:v>-1.752</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.7240000000000002</c:v>
+                  <c:v>-2.7040000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.9670000000000001</c:v>
+                  <c:v>-2.7759999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.9180000000000001</c:v>
+                  <c:v>-2.9209999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.8560000000000001</c:v>
+                  <c:v>-3.177</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.085</c:v>
+                  <c:v>-3.3439999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.5190000000000001</c:v>
+                  <c:v>-3.3210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.3740000000000001</c:v>
+                  <c:v>-3.5150000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.2880000000000003</c:v>
+                  <c:v>-4.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-4.5990000000000002</c:v>
+                  <c:v>-4.4169999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-5.4550000000000001</c:v>
+                  <c:v>-4.43</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-4.6070000000000002</c:v>
+                  <c:v>-5.2169999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.752</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.7589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.7040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.4129999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2.7759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.867</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.3210000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.8119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.5150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2454,32 +2953,32 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>graph!$B$2:$B$13</c:f>
+              <c:f>graph!$B$2:$B$28</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Written Norwegian</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>Natural Sciences</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Religion and Ethics</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social Sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Oral Norwegian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Written English</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oral English</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mathematics</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Natural Sciences</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Social Sciences</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Religion and Ethics</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Music</c:v>
@@ -2488,55 +2987,115 @@
                   <c:v>Arts and Handcraft</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Physical Education</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Food and Health</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Physical Education</c:v>
+                <c:pt idx="13">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>[Exam] Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[Exam] Written English</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[Exam] Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>[Exam] Oral English</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Oral Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>[Exam] Oral Norwegian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$E$2:$E$13</c:f>
+              <c:f>graph!$E$2:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-0.80500000000000005</c:v>
+                  <c:v>-0.13500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.633</c:v>
+                  <c:v>-0.89200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.0169999999999999</c:v>
+                  <c:v>-0.68100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.788</c:v>
+                  <c:v>-1.121</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.21299999999999999</c:v>
+                  <c:v>-1.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.226</c:v>
+                  <c:v>-1.516</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.6379999999999999</c:v>
+                  <c:v>-1.6319999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.583</c:v>
+                  <c:v>-1.494</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.4710000000000001</c:v>
+                  <c:v>-2.319</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.5219999999999998</c:v>
+                  <c:v>-2.3820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.7909999999999999</c:v>
+                  <c:v>-2.8820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-3.0350000000000001</c:v>
+                  <c:v>-2.6320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.13500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.89200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.32600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.68100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.55800000000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.6319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.849</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.494</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.4810000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2576,32 +3135,32 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>graph!$B$2:$B$13</c:f>
+              <c:f>graph!$B$2:$B$28</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Written Norwegian</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>Natural Sciences</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Religion and Ethics</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social Sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Oral Norwegian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Written English</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oral English</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mathematics</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Natural Sciences</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Social Sciences</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Religion and Ethics</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Music</c:v>
@@ -2610,55 +3169,115 @@
                   <c:v>Arts and Handcraft</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Physical Education</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Food and Health</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Physical Education</c:v>
+                <c:pt idx="13">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>[Exam] Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[Exam] Written English</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[Exam] Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>[Exam] Oral English</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Oral Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>[Exam] Oral Norwegian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$F$2:$F$13</c:f>
+              <c:f>graph!$F$2:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>1.2050000000000001</c:v>
+                  <c:v>1.1619999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24199999999999999</c:v>
+                  <c:v>1.0209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95699999999999996</c:v>
+                  <c:v>1.266</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31</c:v>
+                  <c:v>0.41299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.111</c:v>
+                  <c:v>0.23300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34499999999999997</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0999999999999994E-2</c:v>
+                  <c:v>0.38800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.152</c:v>
+                  <c:v>0.32100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.19800000000000001</c:v>
+                  <c:v>-0.11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.14299999999999999</c:v>
+                  <c:v>-5.7000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.33600000000000002</c:v>
+                  <c:v>-0.63400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.73</c:v>
+                  <c:v>-0.24199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.57</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0209999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.526</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.266</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.4940000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.38800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.32100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.14299999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2698,32 +3317,32 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>graph!$B$2:$B$13</c:f>
+              <c:f>graph!$B$2:$B$28</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Written Norwegian</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>Natural Sciences</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Religion and Ethics</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social Sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Oral Norwegian</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Written English</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Oral English</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mathematics</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Natural Sciences</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Social Sciences</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Religion and Ethics</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Music</c:v>
@@ -2732,55 +3351,115 @@
                   <c:v>Arts and Handcraft</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Physical Education</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Food and Health</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Physical Education</c:v>
+                <c:pt idx="13">
+                  <c:v>Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>[Exam] Mathematics</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Written English</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[Exam] Written English</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[Exam] Written Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oral English</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>[Exam] Oral English</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Oral Norwegian</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>[Exam] Oral Norwegian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$G$2:$G$13</c:f>
+              <c:f>graph!$G$2:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>3.605</c:v>
+                  <c:v>3.044</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6219999999999999</c:v>
+                  <c:v>3.153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1379999999999999</c:v>
+                  <c:v>3.613</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6179999999999999</c:v>
+                  <c:v>2.4609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.028</c:v>
+                  <c:v>2.3570000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4329999999999998</c:v>
+                  <c:v>2.3639999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3330000000000002</c:v>
+                  <c:v>2.6419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3250000000000002</c:v>
+                  <c:v>2.6520000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5569999999999999</c:v>
+                  <c:v>2.589</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6869999999999998</c:v>
+                  <c:v>2.7160000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4849999999999999</c:v>
+                  <c:v>2.3039999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2650000000000001</c:v>
+                  <c:v>2.5169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.044</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.464</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.153</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.355</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.613</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3440000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.6419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.6520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.228</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2814,7 +3493,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2829,7 +3508,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2921,7 +3600,17 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.56238054057508036"/>
+          <c:y val="0.63645589107878831"/>
+          <c:w val="0.36507188829110904"/>
+          <c:h val="4.5825167984348193E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4110,16 +4799,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4146,16 +4835,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>42861</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>61911</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4483,7 +5172,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G13" sqref="A1:G13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4799,10 +5488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE763FE5-7F89-44F0-9906-7D9A522CC88D}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4811,594 +5500,587 @@
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="22" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-4.7969999999999997</v>
+      </c>
+      <c r="D2" s="9">
+        <v>-1.752</v>
+      </c>
+      <c r="E2" s="9">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="G2" s="9">
+        <v>3.044</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-4.8230000000000004</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-2.7040000000000002</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-0.89200000000000002</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="G3" s="9">
+        <v>3.153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="14">
-        <v>-5.9530000000000003</v>
-      </c>
-      <c r="D2" s="14">
-        <v>-3.0619999999999998</v>
-      </c>
-      <c r="E2" s="14">
-        <v>-0.80500000000000005</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1.2050000000000001</v>
-      </c>
-      <c r="G2" s="14">
-        <v>3.605</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="C4" s="9">
+        <v>-5.4669999999999996</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-2.7759999999999998</v>
+      </c>
+      <c r="E4" s="9">
+        <v>-0.68100000000000005</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1.266</v>
+      </c>
+      <c r="G4" s="9">
+        <v>3.613</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9">
+        <v>-5.4859999999999998</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-2.9209999999999998</v>
+      </c>
+      <c r="E5" s="9">
+        <v>-1.121</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G5" s="9">
+        <v>2.4609999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-5.5869999999999997</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-3.177</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-1.45</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2.3570000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-5.8449999999999998</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-3.3439999999999999</v>
+      </c>
+      <c r="E7" s="9">
+        <v>-1.516</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2.3639999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-5.3209999999999997</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-3.3210000000000002</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-1.6319999999999999</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="G8" s="9">
+        <v>2.6419999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-6.1109999999999998</v>
+      </c>
+      <c r="D9" s="9">
+        <v>-3.5150000000000001</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-1.494</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="G9" s="9">
+        <v>2.6520000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="9">
+        <v>-6.11</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-4.08</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-2.319</v>
+      </c>
+      <c r="F10" s="9">
+        <v>-0.11</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2.589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-6.2380000000000004</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-4.4169999999999998</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-2.3820000000000001</v>
+      </c>
+      <c r="F11" s="9">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2.7160000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="11">
+        <v>-6.0220000000000002</v>
+      </c>
+      <c r="D12" s="11">
+        <v>-4.43</v>
+      </c>
+      <c r="E12" s="11">
+        <v>-2.8820000000000001</v>
+      </c>
+      <c r="F12" s="11">
+        <v>-0.63400000000000001</v>
+      </c>
+      <c r="G12" s="11">
+        <v>2.3039999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="13">
+        <v>-7.58</v>
+      </c>
+      <c r="D13" s="13">
+        <v>-5.2169999999999996</v>
+      </c>
+      <c r="E13" s="13">
+        <v>-2.6320000000000001</v>
+      </c>
+      <c r="F13" s="13">
+        <v>-0.24199999999999999</v>
+      </c>
+      <c r="G13" s="13">
+        <v>2.5169999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9">
+        <v>-4.7969999999999997</v>
+      </c>
+      <c r="D15" s="9">
+        <v>-1.752</v>
+      </c>
+      <c r="E15" s="9">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="G15" s="9">
+        <v>3.044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="11">
+        <v>-4.8630000000000004</v>
+      </c>
+      <c r="D16" s="11">
+        <v>-1.7589999999999999</v>
+      </c>
+      <c r="E16" s="11">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1.57</v>
+      </c>
+      <c r="G16" s="11">
+        <v>3.464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9">
+        <v>-4.8230000000000004</v>
+      </c>
+      <c r="D18" s="9">
+        <v>-2.7040000000000002</v>
+      </c>
+      <c r="E18" s="9">
+        <v>-0.89200000000000002</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="G18" s="9">
+        <v>3.153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="11">
+        <v>-4.5819999999999999</v>
+      </c>
+      <c r="D19" s="11">
+        <v>-2.4129999999999998</v>
+      </c>
+      <c r="E19" s="11">
+        <v>-0.32600000000000001</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1.526</v>
+      </c>
+      <c r="G19" s="11">
+        <v>3.355</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="9">
+        <v>-5.4669999999999996</v>
+      </c>
+      <c r="D21" s="9">
+        <v>-2.7759999999999998</v>
+      </c>
+      <c r="E21" s="9">
+        <v>-0.68100000000000005</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1.266</v>
+      </c>
+      <c r="G21" s="9">
+        <v>3.613</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="11">
+        <v>-4.7249999999999996</v>
+      </c>
+      <c r="D22" s="11">
+        <v>-1.867</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2.4940000000000002</v>
+      </c>
+      <c r="G22" s="11">
+        <v>4.3440000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="9">
+        <v>-5.3209999999999997</v>
+      </c>
+      <c r="D24" s="9">
+        <v>-3.3210000000000002</v>
+      </c>
+      <c r="E24" s="9">
+        <v>-1.6319999999999999</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="G24" s="9">
+        <v>2.6419999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="11">
+        <v>-5.7030000000000003</v>
+      </c>
+      <c r="D25" s="11">
+        <v>-3.8119999999999998</v>
+      </c>
+      <c r="E25" s="11">
+        <v>-1.849</v>
+      </c>
+      <c r="F25" s="11">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1.2110000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>18</v>
+      <c r="B27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="9">
+        <v>-6.1109999999999998</v>
+      </c>
+      <c r="D27" s="9">
+        <v>-3.5150000000000001</v>
+      </c>
+      <c r="E27" s="9">
+        <v>-1.494</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="G27" s="9">
+        <v>2.6520000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="14">
-        <v>-6.3129999999999997</v>
-      </c>
-      <c r="D3" s="14">
-        <v>-3.7240000000000002</v>
-      </c>
-      <c r="E3" s="14">
-        <v>-1.633</v>
-      </c>
-      <c r="F3" s="14">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="G3" s="14">
-        <v>2.6219999999999999</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-5.1890000000000001</v>
-      </c>
-      <c r="D4" s="10">
-        <v>-2.9670000000000001</v>
-      </c>
-      <c r="E4" s="10">
-        <v>-1.0169999999999999</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="G4" s="10">
-        <v>3.1379999999999999</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="17">
-        <v>-5.9530000000000003</v>
-      </c>
-      <c r="L4" s="17">
-        <v>-6.3129999999999997</v>
-      </c>
-      <c r="M4" s="18">
-        <v>-5.1890000000000001</v>
-      </c>
-      <c r="N4" s="18">
-        <v>-5.6550000000000002</v>
-      </c>
-      <c r="O4" s="17">
-        <v>-4.9340000000000002</v>
-      </c>
-      <c r="P4" s="17">
-        <v>-5.7240000000000002</v>
-      </c>
-      <c r="Q4" s="18">
-        <v>-6.0650000000000004</v>
-      </c>
-      <c r="R4" s="18">
-        <v>-5.8220000000000001</v>
-      </c>
-      <c r="S4" s="17">
-        <v>-6.3049999999999997</v>
-      </c>
-      <c r="T4" s="18">
-        <v>-6.4470000000000001</v>
-      </c>
-      <c r="U4" s="17">
-        <v>-7.7679999999999998</v>
-      </c>
-      <c r="V4" s="18">
-        <v>-6.2210000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-5.6550000000000002</v>
-      </c>
-      <c r="D5" s="10">
-        <v>-3.9180000000000001</v>
-      </c>
-      <c r="E5" s="10">
-        <v>-1.788</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.31</v>
-      </c>
-      <c r="G5" s="10">
-        <v>2.6179999999999999</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="17">
-        <v>-3.0619999999999998</v>
-      </c>
-      <c r="L5" s="17">
-        <v>-3.7240000000000002</v>
-      </c>
-      <c r="M5" s="18">
-        <v>-2.9670000000000001</v>
-      </c>
-      <c r="N5" s="18">
-        <v>-3.9180000000000001</v>
-      </c>
-      <c r="O5" s="17">
-        <v>-1.8560000000000001</v>
-      </c>
-      <c r="P5" s="17">
-        <v>-3.085</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>-3.5190000000000001</v>
-      </c>
-      <c r="R5" s="18">
-        <v>-3.3740000000000001</v>
-      </c>
-      <c r="S5" s="17">
-        <v>-4.2880000000000003</v>
-      </c>
-      <c r="T5" s="18">
-        <v>-4.5990000000000002</v>
-      </c>
-      <c r="U5" s="17">
-        <v>-5.4550000000000001</v>
-      </c>
-      <c r="V5" s="18">
-        <v>-4.6070000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="14">
-        <v>-4.9340000000000002</v>
-      </c>
-      <c r="D6" s="14">
-        <v>-1.8560000000000001</v>
-      </c>
-      <c r="E6" s="14">
-        <v>-0.21299999999999999</v>
-      </c>
-      <c r="F6" s="14">
-        <v>1.111</v>
-      </c>
-      <c r="G6" s="14">
-        <v>3.028</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="17">
-        <v>-0.80500000000000005</v>
-      </c>
-      <c r="L6" s="17">
-        <v>-1.633</v>
-      </c>
-      <c r="M6" s="18">
-        <v>-1.0169999999999999</v>
-      </c>
-      <c r="N6" s="18">
-        <v>-1.788</v>
-      </c>
-      <c r="O6" s="17">
-        <v>-0.21299999999999999</v>
-      </c>
-      <c r="P6" s="17">
-        <v>-1.226</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>-1.6379999999999999</v>
-      </c>
-      <c r="R6" s="18">
-        <v>-1.583</v>
-      </c>
-      <c r="S6" s="17">
-        <v>-2.4710000000000001</v>
-      </c>
-      <c r="T6" s="18">
-        <v>-2.5219999999999998</v>
-      </c>
-      <c r="U6" s="17">
-        <v>-2.7909999999999999</v>
-      </c>
-      <c r="V6" s="18">
-        <v>-3.0350000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="14">
-        <v>-5.7240000000000002</v>
-      </c>
-      <c r="D7" s="14">
-        <v>-3.085</v>
-      </c>
-      <c r="E7" s="14">
-        <v>-1.226</v>
-      </c>
-      <c r="F7" s="14">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="G7" s="14">
-        <v>2.4329999999999998</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="17">
-        <v>1.2050000000000001</v>
-      </c>
-      <c r="L7" s="17">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="M7" s="18">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="N7" s="18">
-        <v>0.31</v>
-      </c>
-      <c r="O7" s="17">
-        <v>1.111</v>
-      </c>
-      <c r="P7" s="17">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="R7" s="18">
-        <v>0.152</v>
-      </c>
-      <c r="S7" s="17">
-        <v>-0.19800000000000001</v>
-      </c>
-      <c r="T7" s="18">
-        <v>-0.14299999999999999</v>
-      </c>
-      <c r="U7" s="17">
-        <v>-0.33600000000000002</v>
-      </c>
-      <c r="V7" s="18">
-        <v>-0.73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-6.0650000000000004</v>
-      </c>
-      <c r="D8" s="10">
-        <v>-3.5190000000000001</v>
-      </c>
-      <c r="E8" s="10">
-        <v>-1.6379999999999999</v>
-      </c>
-      <c r="F8" s="10">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="G8" s="10">
-        <v>2.3330000000000002</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="17">
-        <v>3.605</v>
-      </c>
-      <c r="L8" s="17">
-        <v>2.6219999999999999</v>
-      </c>
-      <c r="M8" s="18">
-        <v>3.1379999999999999</v>
-      </c>
-      <c r="N8" s="18">
-        <v>2.6179999999999999</v>
-      </c>
-      <c r="O8" s="17">
-        <v>3.028</v>
-      </c>
-      <c r="P8" s="17">
-        <v>2.4329999999999998</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>2.3330000000000002</v>
-      </c>
-      <c r="R8" s="18">
-        <v>2.3250000000000002</v>
-      </c>
-      <c r="S8" s="17">
-        <v>2.5569999999999999</v>
-      </c>
-      <c r="T8" s="18">
-        <v>2.6869999999999998</v>
-      </c>
-      <c r="U8" s="17">
-        <v>2.4849999999999999</v>
-      </c>
-      <c r="V8" s="18">
-        <v>2.2650000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="10">
-        <v>-5.8220000000000001</v>
-      </c>
-      <c r="D9" s="10">
-        <v>-3.3740000000000001</v>
-      </c>
-      <c r="E9" s="10">
-        <v>-1.583</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0.152</v>
-      </c>
-      <c r="G9" s="10">
-        <v>2.3250000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="14">
-        <v>-6.3049999999999997</v>
-      </c>
-      <c r="D10" s="14">
-        <v>-4.2880000000000003</v>
-      </c>
-      <c r="E10" s="14">
-        <v>-2.4710000000000001</v>
-      </c>
-      <c r="F10" s="14">
-        <v>-0.19800000000000001</v>
-      </c>
-      <c r="G10" s="14">
-        <v>2.5569999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="10">
-        <v>-6.4470000000000001</v>
-      </c>
-      <c r="D11" s="10">
-        <v>-4.5990000000000002</v>
-      </c>
-      <c r="E11" s="10">
-        <v>-2.5219999999999998</v>
-      </c>
-      <c r="F11" s="10">
-        <v>-0.14299999999999999</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2.6869999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="14">
-        <v>-7.7679999999999998</v>
-      </c>
-      <c r="D12" s="14">
-        <v>-5.4550000000000001</v>
-      </c>
-      <c r="E12" s="14">
-        <v>-2.7909999999999999</v>
-      </c>
-      <c r="F12" s="14">
-        <v>-0.33600000000000002</v>
-      </c>
-      <c r="G12" s="14">
-        <v>2.4849999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="11">
-        <v>-6.2210000000000001</v>
-      </c>
-      <c r="D13" s="11">
-        <v>-4.6070000000000002</v>
-      </c>
-      <c r="E13" s="11">
-        <v>-3.0350000000000001</v>
-      </c>
-      <c r="F13" s="11">
-        <v>-0.73</v>
-      </c>
-      <c r="G13" s="11">
-        <v>2.2650000000000001</v>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="13">
+        <v>-6.0060000000000002</v>
+      </c>
+      <c r="D28" s="13">
+        <v>-3.516</v>
+      </c>
+      <c r="E28" s="13">
+        <v>-1.4810000000000001</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G28" s="13">
+        <v>1.228</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G19">
+    <sortCondition descending="1" ref="E4:E19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>